<commit_message>
update System test rerport
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE28723-FA94-49FA-A545-4B0FB3072BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Test Report" sheetId="2" r:id="rId1"/>
     <sheet name="Test Cases &amp; Results" sheetId="1" r:id="rId2"/>
     <sheet name="Enums" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -20,6 +21,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -83,30 +86,365 @@
     <t>Low Impact</t>
   </si>
   <si>
-    <t>Test that the water heater is activated if the water temperature is &lt; 100 Deg C</t>
-  </si>
-  <si>
-    <t>Water temperature is &lt; 100 Deg C</t>
-  </si>
-  <si>
-    <t>From the LCD main menu, select the option "Black Coffee"</t>
-  </si>
-  <si>
-    <t>-Heating element is activated when water temperature is &lt; 100 Deg C</t>
+    <t>REQ-04</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-05</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>REQ-06</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-07</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-15</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>High Impact</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mid Impact</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that the RPI prompts to scan the user's IC, displays "Scan your IC" on the LCD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that the LCD displays the location and the prompt “Press ‘*’”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>System is powered on and ready</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays "Scan your IC" and the camera activates</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that if the barcode corresponds to an account, the user's name and admin number are displayed on the LCD for 1 second</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valid barcode for an existing account</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays the user's name and admin number for 1 second</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that if the barcode does not correspond to an account, the LCD displays “Please press ‘#’ to try again”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalid barcode</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “Please press ‘#’ to try again”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>User has logged into the system</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays "Location [1 or 2]" and "Press ‘*’"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-08</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that the LCD displays the main menu options and rotates through the screens</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays and rotates through the menu options</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-09</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that if "Collect" is selected, the location is checked, and if correct, the book is dispensed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>User has selected the "Collect" option and is at the correct location</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The book is dispensed if the user is at the correct location</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-10</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that if "Collect" is selected and the location is incorrect, the LCD displays “Wrong location. Go to location [1/2]”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>User has selected the "Collect" option and is at the wrong location</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “Wrong location. Go to location [1/2]”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-11</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that if more than 10 books have been collected, the system stops dispensing books and the LCD displays “Maximum books reached (10)”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>User has already collected 10 books</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “Maximum books reached (10)”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that when option 3 is pressed, the LCD displays “Which book to extend loan”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>User is on the main menu and selects option 3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “Which book to extend loan”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-16</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that the respective names for the lent books are displayed on the LCD, cycling through them if there is more than one book</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>User has lent books</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD cycles through and displays the names of the lent books</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-17</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that if the selected book has not been extended before, the LCD displays “Successfully extended loan”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>User selects a book that has not been extended before</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “Successfully extended loan”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-18</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that if the selected book has been extended before, the LCD displays “Previously extended”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>User selects a book that has been extended before</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “Previously extended”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-19</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that when option 4 is pressed, the LCD displays “Scan your card to pay fine” and activates the RFID scanner</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>User is on the main menu and selects option 4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “Scan your card to pay fine” and the RFID scanner activates</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-20</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that users with unpaid fines are not allowed to borrow any books</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>User has unpaid fines</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The system prevents borrowing and displays an appropriate message if there are unpaid fines</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-21</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that if there are no fines, the LCD displays “No fines” before ending the session and returning to the main page</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>User has no unpaid fines</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “No fines” and returns to the main page</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Scan an invalid barcode  2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Attempt to check fines  2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Start the system              2. Check the LCD display</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Scan a valid barcode     2. Check the LCD display</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Navigate to the main menu                                                2. Check the LCD display</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Select the "Collect" option                                                  2. Verify location                                                       3. Check if the book is dispensed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Select the "Collect" option                                               2. Verify location                               3. Check the LCD display</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Attempt to collect an 11th book                                              2. Check the LCD display</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Press option 3                             2. Check the LCD display</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Navigate to the loan extension menu                             2. Check the LCD display</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Select a book that has not been extended                            2. Check the LCD display</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Select a book that has been extended                               2. Check the LCD display</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Press option 4                              2. Check the LCD display  3. Check the RFID scanner activation</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Attempt to borrow a book                                        2. Check the LCD display</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “No fines” and returns to the main page</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Scan your card to pay fine” and the RFID scanner activates</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Previously extended”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Successfully extended loan”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD cycles through and displays the names of the lent books</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Which book to extend loan”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Maximum books reached (10)”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Wrong location. Go to location [1/2]”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays and rotates through the menu options</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Please press ‘#’ to try again”</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays the user's name and admin number for 1 second</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays "Scan your IC" and the camera activates</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays "Location [1 or 2]" and "Press ‘*’"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -114,7 +452,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -123,6 +461,20 @@
       <color rgb="FF333333"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="7">
@@ -190,21 +542,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -221,22 +561,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -248,13 +580,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -274,7 +599,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -311,7 +636,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -337,7 +661,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -487,13 +811,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -559,13 +883,12 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -573,6 +896,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -596,7 +920,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1208,9 +1532,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1248,9 +1572,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1285,7 +1609,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1320,7 +1644,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1493,55 +1817,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C6"/>
   <sheetViews>
     <sheetView zoomScale="129" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!B3:B70, "&lt;&gt;")</f>
-        <v>20</v>
+      <c r="C3" s="6">
+        <f>COUNTIF('Test Cases &amp; Results'!B3:B65, "&lt;&gt;")</f>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Pass")</f>
-        <v>1</v>
+      <c r="C4" s="6">
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K67, "Pass")</f>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Fail")</f>
+      <c r="C5" s="6">
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K67, "Fail")</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Not Tested")</f>
-        <v>19</v>
+      <c r="C6" s="6">
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K67, "Not Tested")</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1549,25 +1874,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18:K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="28.1796875" customWidth="1"/>
+    <col min="7" max="7" width="21.7265625" customWidth="1"/>
+    <col min="8" max="8" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.453125" customWidth="1"/>
+    <col min="10" max="10" width="18.54296875" customWidth="1"/>
+    <col min="11" max="11" width="12.54296875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
@@ -1598,384 +1923,495 @@
       <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+      <c r="B3" s="10">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="10">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="15" t="s">
+      <c r="D3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="12" t="s">
+      <c r="E3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="K3" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+    <row r="4" spans="2:11" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="10">
         <f>B3+1</f>
         <v>2</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="12" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="10">
+        <f t="shared" ref="B5:B17" si="0">B4+1</f>
         <v>3</v>
       </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <f t="shared" ref="B5:B20" si="0">B4+1</f>
-        <v>3</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
+    <row r="6" spans="2:11" ht="66" x14ac:dyDescent="0.25">
+      <c r="B6" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="12" t="s">
-        <v>3</v>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
+    <row r="7" spans="2:11" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="12" t="s">
-        <v>3</v>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
+    <row r="8" spans="2:11" ht="66" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="12" t="s">
-        <v>3</v>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
+    <row r="9" spans="2:11" ht="66" x14ac:dyDescent="0.25">
+      <c r="B9" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="12" t="s">
-        <v>3</v>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
+    <row r="10" spans="2:11" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="12" t="s">
-        <v>3</v>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
+    <row r="11" spans="2:11" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="12" t="s">
-        <v>3</v>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
+    <row r="12" spans="2:11" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="12" t="s">
-        <v>3</v>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
+    <row r="13" spans="2:11" ht="66" x14ac:dyDescent="0.25">
+      <c r="B13" s="10">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="12" t="s">
-        <v>3</v>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
+    <row r="14" spans="2:11" ht="66" x14ac:dyDescent="0.25">
+      <c r="B14" s="10">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="12" t="s">
-        <v>3</v>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
+    <row r="15" spans="2:11" ht="66" x14ac:dyDescent="0.25">
+      <c r="B15" s="10">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="12" t="s">
-        <v>3</v>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
+    <row r="16" spans="2:11" ht="99" x14ac:dyDescent="0.25">
+      <c r="B16" s="10">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="12" t="s">
-        <v>3</v>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
+    <row r="17" spans="2:11" ht="66" x14ac:dyDescent="0.25">
+      <c r="B17" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="12" t="s">
-        <v>3</v>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
-        <f t="shared" ref="B21:B22" si="1">B20+1</f>
-        <v>19</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="2">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="12" t="s">
-        <v>3</v>
-      </c>
+    <row r="18" spans="2:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K3:K20">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K20">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="K3:K17">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:K22">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:K22">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1983,17 +2419,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Enums!$B$8:$B$10</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E5</xm:sqref>
+          <xm:sqref>E4:E6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Enums!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K22</xm:sqref>
+          <xm:sqref>K3:K17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2002,14 +2438,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -2042,24 +2478,25 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2221,6 +2658,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2232,14 +2677,6 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
edited test report font
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE28723-FA94-49FA-A545-4B0FB3072BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7E06B4-82E4-4CFE-891A-959EBC0ED733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Test Report" sheetId="2" r:id="rId1"/>
@@ -87,247 +87,247 @@
   </si>
   <si>
     <t>REQ-04</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-05</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-06</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-07</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-15</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>High Impact</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Mid Impact</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that the RPI prompts to scan the user's IC, displays "Scan your IC" on the LCD</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that the LCD displays the location and the prompt “Press ‘*’”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>System is powered on and ready</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The LCD displays "Scan your IC" and the camera activates</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that if the barcode corresponds to an account, the user's name and admin number are displayed on the LCD for 1 second</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Valid barcode for an existing account</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The LCD displays the user's name and admin number for 1 second</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that if the barcode does not correspond to an account, the LCD displays “Please press ‘#’ to try again”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Invalid barcode</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The LCD displays “Please press ‘#’ to try again”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>User has logged into the system</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The LCD displays "Location [1 or 2]" and "Press ‘*’"</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-08</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that the LCD displays the main menu options and rotates through the screens</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The LCD displays and rotates through the menu options</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-09</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that if "Collect" is selected, the location is checked, and if correct, the book is dispensed</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>User has selected the "Collect" option and is at the correct location</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The book is dispensed if the user is at the correct location</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-10</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that if "Collect" is selected and the location is incorrect, the LCD displays “Wrong location. Go to location [1/2]”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>User has selected the "Collect" option and is at the wrong location</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The LCD displays “Wrong location. Go to location [1/2]”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-11</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that if more than 10 books have been collected, the system stops dispensing books and the LCD displays “Maximum books reached (10)”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>User has already collected 10 books</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The LCD displays “Maximum books reached (10)”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that when option 3 is pressed, the LCD displays “Which book to extend loan”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>User is on the main menu and selects option 3</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The LCD displays “Which book to extend loan”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-16</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that the respective names for the lent books are displayed on the LCD, cycling through them if there is more than one book</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>User has lent books</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The LCD cycles through and displays the names of the lent books</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-17</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that if the selected book has not been extended before, the LCD displays “Successfully extended loan”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>User selects a book that has not been extended before</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The LCD displays “Successfully extended loan”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-18</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that if the selected book has been extended before, the LCD displays “Previously extended”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>User selects a book that has been extended before</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The LCD displays “Previously extended”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-19</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that when option 4 is pressed, the LCD displays “Scan your card to pay fine” and activates the RFID scanner</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>User is on the main menu and selects option 4</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The LCD displays “Scan your card to pay fine” and the RFID scanner activates</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-20</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that users with unpaid fines are not allowed to borrow any books</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>User has unpaid fines</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The system prevents borrowing and displays an appropriate message if there are unpaid fines</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-21</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that if there are no fines, the LCD displays “No fines” before ending the session and returning to the main page</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>User has no unpaid fines</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The LCD displays “No fines” and returns to the main page</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1. Scan an invalid barcode  2. Check the LCD display</t>
@@ -337,114 +337,114 @@
   </si>
   <si>
     <t>1. Start the system              2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1. Scan a valid barcode     2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1. Navigate to the main menu                                                2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1. Select the "Collect" option                                                  2. Verify location                                                       3. Check if the book is dispensed</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1. Select the "Collect" option                                               2. Verify location                               3. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1. Attempt to collect an 11th book                                              2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1. Press option 3                             2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1. Navigate to the loan extension menu                             2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1. Select a book that has not been extended                            2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1. Select a book that has been extended                               2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1. Press option 4                              2. Check the LCD display  3. Check the RFID scanner activation</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1. Attempt to borrow a book                                        2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>LCD displays “No fines” and returns to the main page</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>LCD displays “Scan your card to pay fine” and the RFID scanner activates</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>LCD displays “Previously extended”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>LCD displays “Successfully extended loan”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>LCD cycles through and displays the names of the lent books</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>LCD displays “Which book to extend loan”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>LCD displays “Maximum books reached (10)”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>LCD displays “Wrong location. Go to location [1/2]”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>LCD displays and rotates through the menu options</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>LCD displays “Please press ‘#’ to try again”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>LCD displays the user's name and admin number for 1 second</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>LCD displays "Scan your IC" and the camera activates</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>LCD displays "Location [1 or 2]" and "Press ‘*’"</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -452,19 +452,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FF333333"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -475,6 +469,13 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -542,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -555,18 +556,21 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -599,7 +603,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -661,7 +665,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -883,7 +887,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -920,7 +924,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1820,16 +1824,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView zoomScale="129" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1838,7 +1842,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1847,7 +1851,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1856,7 +1860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1866,7 +1870,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1877,25 +1881,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18:K22"/>
+    <sheetView topLeftCell="A11" zoomScale="84" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="28.1796875" customWidth="1"/>
-    <col min="7" max="7" width="21.7265625" customWidth="1"/>
-    <col min="8" max="8" width="25.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.453125" customWidth="1"/>
-    <col min="10" max="10" width="18.54296875" customWidth="1"/>
-    <col min="11" max="11" width="12.54296875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="28.21875" customWidth="1"/>
+    <col min="7" max="7" width="21.77734375" customWidth="1"/>
+    <col min="8" max="8" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" customWidth="1"/>
+    <col min="10" max="10" width="18.5546875" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1927,7 +1931,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="57" customHeight="1">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -1955,11 +1959,11 @@
       <c r="J3" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="43.2">
       <c r="B4" s="10">
         <f>B3+1</f>
         <v>2</v>
@@ -1986,11 +1990,11 @@
       <c r="J4" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="72">
       <c r="B5" s="10">
         <f t="shared" ref="B5:B17" si="0">B4+1</f>
         <v>3</v>
@@ -2017,11 +2021,11 @@
       <c r="J5" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="66" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="57.6">
       <c r="B6" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2048,11 +2052,11 @@
       <c r="J6" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="43.2">
       <c r="B7" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2079,11 +2083,11 @@
       <c r="J7" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="66" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="57.6">
       <c r="B8" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2110,11 +2114,11 @@
       <c r="J8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="66" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="57.6">
       <c r="B9" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2141,11 +2145,11 @@
       <c r="J9" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="72">
       <c r="B10" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2172,11 +2176,11 @@
       <c r="J10" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="43.2">
       <c r="B11" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2203,11 +2207,11 @@
       <c r="J11" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="57.6">
       <c r="B12" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2234,11 +2238,11 @@
       <c r="J12" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="66" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="57.6">
       <c r="B13" s="10">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2265,11 +2269,11 @@
       <c r="J13" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="66" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="57.6">
       <c r="B14" s="10">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2296,11 +2300,11 @@
       <c r="J14" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="K14" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="66" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="57.6">
       <c r="B15" s="10">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2327,11 +2331,11 @@
       <c r="J15" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K15" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="99" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" ht="86.4">
       <c r="B16" s="10">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2358,11 +2362,11 @@
       <c r="J16" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K16" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="66" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="57.6">
       <c r="B17" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2389,23 +2393,23 @@
       <c r="J17" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="K17" s="8" t="s">
+      <c r="K17" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
+    <row r="18" spans="2:11">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="K3:K17">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
@@ -2445,61 +2449,46 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2">
       <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2">
       <c r="B3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2">
       <c r="B8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2">
       <c r="B9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2">
       <c r="B10" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E81D8C8DDAE8BD44A422697963F06C45" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6816e004dbb89c674e51f5647972552">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2b02348f-b4e3-458c-83fc-9e90db0f8029" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6418ca14ac9ee17b8bbf6df78e0c223" ns2:_="">
     <xsd:import namespace="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
@@ -2657,10 +2646,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCDB6385-31B2-4574-9AA4-BF13B563A4E3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2682,19 +2696,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCDB6385-31B2-4574-9AA4-BF13B563A4E3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated system test files
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7E06B4-82E4-4CFE-891A-959EBC0ED733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8791C450-4F71-402C-AEFD-6027D56F203F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Test Report" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="139">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -134,10 +134,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Valid barcode for an existing account</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>The LCD displays the user's name and admin number for 1 second</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -146,294 +142,426 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Invalid barcode</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>The LCD displays “Please press ‘#’ to try again”</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>The LCD displays "Location [1 or 2]" and "Press ‘*’"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-08</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that the LCD displays the main menu options and rotates through the screens</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-09</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “Wrong location. Go to location [1/2]”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-11</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “Maximum books reached (10)”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “Which book to extend loan”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-16</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that the respective names for the lent books are displayed on the LCD, cycling through them if there is more than one book</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD cycles through and displays the names of the lent books</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-17</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “Successfully extended loan”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-18</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that if the selected book has been extended before, the LCD displays “Previously extended”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-19</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “Scan your card to pay fine” and the RFID scanner activates</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that users with unpaid fines are not allowed to borrow any books</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-21</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Scan your card to pay fine” and the RFID scanner activates</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Previously extended”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Successfully extended loan”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD cycles through and displays the names of the lent books</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Which book to extend loan”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Maximum books reached (10)”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Wrong location. Go to location [1/2]”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays and rotates through the menu options</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Please press ‘#’ to try again”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays the user's name and admin number for 1 second</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays "Scan your IC" and the camera activates</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays "Location [1 or 2]" and "Press ‘*’"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-02</t>
+  </si>
+  <si>
+    <t>Test that the location changes when switch state is changed</t>
+  </si>
+  <si>
+    <t>The LCD displays "Location 1" on line 1 which changes to "Location 2"</t>
+  </si>
+  <si>
+    <t>1. Start the system 
+2. Ensure that the switch is in the left position
+3. Flip the switch to the right position
+4. Check the LCD display</t>
+  </si>
+  <si>
+    <t>System is powered on and ready</t>
+  </si>
+  <si>
+    <t>1. Start the system     
+2. Press '*' on the keypad       
+3. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Place a valid barcode in front of the camera
+2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Place an invalid barcode or no barcode in front of the camera
+2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>Camera is activated and scanning for a barcode</t>
+  </si>
+  <si>
+    <t>1. Check the LCD display</t>
+  </si>
+  <si>
+    <r>
+      <t>The servo motor rotates to 90</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>̊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The DC motor rotates for 5s
+The servo motor rotates to 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>̊</t>
+    </r>
+  </si>
+  <si>
+    <t>Test that when option 3 is pressed, the LCD displays “Which book to extend loan”</t>
+  </si>
+  <si>
+    <t>Test that if more than 10 books have been collected, the system stops dispensing books and the LCD displays “Maximum books reached (10)”</t>
+  </si>
+  <si>
+    <t>Test that if "Collect" is selected and the location is incorrect, the LCD displays “Wrong location. Go to location [1/2]”</t>
+  </si>
+  <si>
+    <t>Test that if "Collect" is selected, the location is checked, and if correct, the book is dispensed</t>
+  </si>
+  <si>
+    <t>1. Press '1' on the keypad  
+2. Verify location is the same location
+3. Check if the motor turn sequence activates, signifying a book being dispensed</t>
+  </si>
+  <si>
+    <t>1. Attempt to collect an 11th book                                              2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Press '3' on the keypad 
+2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Select a book that has not been extended
+2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Select a book that has been extended
+2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Press '4' on the keypad 
+2. Check the LCD display 
+3. Check the RFID scanner activation</t>
+  </si>
+  <si>
+    <t>1. Attempt to borrow a book
+2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Attempt to check fines 
+2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Start the system
+2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>The LCD displays “Previously extended”</t>
+  </si>
+  <si>
+    <t>REQ-26</t>
+  </si>
+  <si>
+    <t>REQ-25</t>
+  </si>
+  <si>
+    <t>Test that if waiting 1min, the program returns to the home page</t>
+  </si>
+  <si>
+    <t>Test that when option 4 is pressed, the LCD displays “Scan your card to pay fine” and activates the RFID scanner</t>
+  </si>
+  <si>
+    <t>Test that when option 5 is pressed, the program returns to the home page</t>
+  </si>
+  <si>
+    <t>User has logged into the system and is at the options page</t>
+  </si>
+  <si>
     <t>User has logged into the system</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD displays "Location [1 or 2]" and "Press ‘*’"</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-08</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that the LCD displays the main menu options and rotates through the screens</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">User has borrowed a book at a location
+User has logged into the system
+</t>
+  </si>
+  <si>
+    <t>1. Press '1' on the keypad 
+2. Verify location is the other location
+3. Check the LCD</t>
+  </si>
+  <si>
+    <t>User has already collected 10 books
+User has logged into the system</t>
+  </si>
+  <si>
+    <t>User has borrowed books
+User has logged into the system</t>
+  </si>
+  <si>
+    <t>User selects a book that has not been extended before
+User has logged into the system and pressed option 3</t>
+  </si>
+  <si>
+    <t>User selects a book that has been extended before
+User has logged into the system and pressed option 3</t>
+  </si>
+  <si>
+    <t>User has unpaid fines
+User has logged into the system</t>
+  </si>
+  <si>
+    <t>User has no unpaid fines
+User has logged into the system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Press '5' on the keypad 
+2. Check the LCD display </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Wait for 1 minute 
+2. Check the LCD display </t>
+  </si>
+  <si>
+    <t>LCD displays “Time out” and returns to the home page</t>
+  </si>
+  <si>
+    <t>LCD displays “No fine incurred” and returns to the options page</t>
+  </si>
+  <si>
+    <t>LCD displays “Pls pay fine first” and returns to the options page</t>
   </si>
   <si>
     <t>The LCD displays and rotates through the menu options</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-09</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that if "Collect" is selected, the location is checked, and if correct, the book is dispensed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>User has selected the "Collect" option and is at the correct location</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The book is dispensed if the user is at the correct location</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that if "Collect" is selected and the location is incorrect, the LCD displays “Wrong location. Go to location [1/2]”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>User has selected the "Collect" option and is at the wrong location</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD displays “Wrong location. Go to location [1/2]”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-11</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that if more than 10 books have been collected, the system stops dispensing books and the LCD displays “Maximum books reached (10)”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>User has already collected 10 books</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD displays “Maximum books reached (10)”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that when option 3 is pressed, the LCD displays “Which book to extend loan”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>User is on the main menu and selects option 3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD displays “Which book to extend loan”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-16</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that the respective names for the lent books are displayed on the LCD, cycling through them if there is more than one book</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>User has lent books</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD cycles through and displays the names of the lent books</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-17</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that if there are no fines, the LCD displays “No fines” before ending the session and returning to the options page</t>
+  </si>
+  <si>
+    <t>LCD returns to the home page</t>
+  </si>
+  <si>
+    <t>REQ-03</t>
+  </si>
+  <si>
+    <t>REQ-01</t>
+  </si>
+  <si>
+    <t>REQ-12</t>
+  </si>
+  <si>
+    <t>REQ-13</t>
+  </si>
+  <si>
+    <t>REQ-14</t>
+  </si>
+  <si>
+    <t>Test that the webpage can be accessed and brings user to sign in page</t>
+  </si>
+  <si>
+    <t>1. Go to IP of the webpage</t>
+  </si>
+  <si>
+    <t>The webpage brings user to the sign in page</t>
+  </si>
+  <si>
+    <t>Internet connected is enabled
+User has not signed in on the webpage</t>
+  </si>
+  <si>
+    <t>Test that the location can be chosen while reserving book</t>
+  </si>
+  <si>
+    <t>1. Go to IP of the webpage
+2. Reserve a book</t>
+  </si>
+  <si>
+    <t>The option of reserving at Location 1 or Location 2 is present</t>
+  </si>
+  <si>
+    <t>The LCD displays borrowed books which can be chosen to return</t>
+  </si>
+  <si>
+    <t>Test that if "Return" is selected, the location is checked, and if correct, the book is dispensed</t>
+  </si>
+  <si>
+    <t>Test that reserved books are automatically removed after 5 days</t>
   </si>
   <si>
     <t>Test that if the selected book has not been extended before, the LCD displays “Successfully extended loan”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>User selects a book that has not been extended before</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD displays “Successfully extended loan”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-18</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that if the selected book has been extended before, the LCD displays “Previously extended”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>User selects a book that has been extended before</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD displays “Previously extended”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-19</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that when option 4 is pressed, the LCD displays “Scan your card to pay fine” and activates the RFID scanner</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>User is on the main menu and selects option 4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD displays “Scan your card to pay fine” and the RFID scanner activates</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-20</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that users with unpaid fines are not allowed to borrow any books</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>User has unpaid fines</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The system prevents borrowing and displays an appropriate message if there are unpaid fines</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-21</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that if there are no fines, the LCD displays “No fines” before ending the session and returning to the main page</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>User has no unpaid fines</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD displays “No fines” and returns to the main page</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Scan an invalid barcode  2. Check the LCD display</t>
-  </si>
-  <si>
-    <t>1. Attempt to check fines  2. Check the LCD display</t>
-  </si>
-  <si>
-    <t>1. Start the system              2. Check the LCD display</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Scan a valid barcode     2. Check the LCD display</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Navigate to the main menu                                                2. Check the LCD display</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Select the "Collect" option                                                  2. Verify location                                                       3. Check if the book is dispensed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Select the "Collect" option                                               2. Verify location                               3. Check the LCD display</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Attempt to collect an 11th book                                              2. Check the LCD display</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Press option 3                             2. Check the LCD display</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Navigate to the loan extension menu                             2. Check the LCD display</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Select a book that has not been extended                            2. Check the LCD display</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Select a book that has been extended                               2. Check the LCD display</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Press option 4                              2. Check the LCD display  3. Check the RFID scanner activation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Attempt to borrow a book                                        2. Check the LCD display</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays “No fines” and returns to the main page</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays “Scan your card to pay fine” and the RFID scanner activates</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays “Previously extended”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays “Successfully extended loan”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD cycles through and displays the names of the lent books</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays “Which book to extend loan”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays “Maximum books reached (10)”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays “Wrong location. Go to location [1/2]”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays and rotates through the menu options</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays “Please press ‘#’ to try again”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays the user's name and admin number for 1 second</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays "Scan your IC" and the camera activates</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays "Location [1 or 2]" and "Press ‘*’"</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">User has reserved a book at a location
+User has logged into the system
+</t>
+  </si>
+  <si>
+    <t>Test that fines are automatically calculated after 18 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User has reserved a book
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User has borrowed a book
+</t>
+  </si>
+  <si>
+    <t>[Software Unit Test]</t>
+  </si>
+  <si>
+    <t>REQ-22</t>
+  </si>
+  <si>
+    <t>REQ-23</t>
+  </si>
+  <si>
+    <t>REQ-24</t>
+  </si>
+  <si>
+    <t>[Non-functional Req]</t>
   </si>
 </sst>
 </file>
@@ -464,18 +592,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -559,14 +686,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -815,13 +942,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1824,7 +1951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
+    <sheetView zoomScale="129" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1838,8 +1965,8 @@
         <v>0</v>
       </c>
       <c r="C3" s="6">
-        <f>COUNTIF('Test Cases &amp; Results'!B3:B65, "&lt;&gt;")</f>
-        <v>15</v>
+        <f>COUNTIF('Test Cases &amp; Results'!B3:B66, "&lt;&gt;")</f>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -1847,8 +1974,8 @@
         <v>1</v>
       </c>
       <c r="C4" s="6">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K67, "Pass")</f>
-        <v>15</v>
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K68, "Pass")</f>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:3">
@@ -1856,7 +1983,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="6">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K67, "Fail")</f>
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K68, "Fail")</f>
         <v>0</v>
       </c>
     </row>
@@ -1865,8 +1992,8 @@
         <v>3</v>
       </c>
       <c r="C6" s="6">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K67, "Not Tested")</f>
-        <v>0</v>
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K68, "Not Tested")</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1879,10 +2006,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:K18"/>
+  <dimension ref="B2:K28"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="84" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="129" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1895,7 +2022,7 @@
     <col min="7" max="7" width="21.77734375" customWidth="1"/>
     <col min="8" max="8" width="25.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.44140625" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" customWidth="1"/>
     <col min="11" max="11" width="12.5546875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1931,486 +2058,753 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="57" customHeight="1">
-      <c r="B3" s="10">
+    <row r="3" spans="2:11" ht="57.6">
+      <c r="B3" s="9">
         <v>1</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>1</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="86.4">
+      <c r="B4" s="9">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="57.6">
+      <c r="B5" s="9">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="43.2">
+      <c r="B6" s="9">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="72">
+      <c r="B7" s="9">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="57.6">
+      <c r="B8" s="9">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="102.6" customHeight="1">
+      <c r="B9" s="9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G9" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="83.4" customHeight="1">
+      <c r="B10" s="9">
+        <v>8</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="G10" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="100.8">
+      <c r="B11" s="9">
+        <v>9</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="86.4">
+      <c r="B12" s="9">
+        <v>10</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="72">
+      <c r="B13" s="9">
+        <v>11</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="86.4">
+      <c r="B14" s="9">
+        <v>12</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="43.2">
+      <c r="B15" s="9">
+        <v>13</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="43.2">
+      <c r="B16" s="9">
+        <v>14</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="43.2">
+      <c r="B17" s="9">
+        <v>15</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="10" t="s">
+      <c r="I17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="72">
+      <c r="B18" s="9">
+        <v>16</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="86.4">
+      <c r="B19" s="9">
+        <v>17</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="86.4">
+      <c r="B20" s="9">
+        <v>18</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="57.6">
+      <c r="B21" s="9">
+        <v>19</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="57.6">
+      <c r="B22" s="9">
+        <v>20</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="57.6">
+      <c r="B23" s="9">
+        <v>21</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="H23" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="K23" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="43.2">
-      <c r="B4" s="10">
-        <f>B3+1</f>
-        <v>2</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="10" t="s">
+    <row r="24" spans="2:11">
+      <c r="B24" s="9">
+        <v>22</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11">
+      <c r="B25" s="9">
         <v>23</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="D25" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11">
+      <c r="B26" s="9">
+        <v>24</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="43.2">
+      <c r="B27" s="9">
         <v>25</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="K4" s="11" t="s">
+      <c r="D27" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="K27" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="72">
-      <c r="B5" s="10">
-        <f t="shared" ref="B5:B17" si="0">B4+1</f>
-        <v>3</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="K5" s="11" t="s">
+    <row r="28" spans="2:11" ht="43.2">
+      <c r="B28" s="9">
+        <v>26</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="K28" s="10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" ht="57.6">
-      <c r="B6" s="10">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" ht="43.2">
-      <c r="B7" s="10">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="57.6">
-      <c r="B8" s="10">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="57.6">
-      <c r="B9" s="10">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="72">
-      <c r="B10" s="10">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="43.2">
-      <c r="B11" s="10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="57.6">
-      <c r="B12" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="57.6">
-      <c r="B13" s="10">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" ht="57.6">
-      <c r="B14" s="10">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" ht="57.6">
-      <c r="B15" s="10">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" ht="86.4">
-      <c r="B16" s="10">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" ht="57.6">
-      <c r="B17" s="10">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11">
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="K3:K17">
+  <conditionalFormatting sqref="K3:K28">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
@@ -2427,13 +2821,13 @@
           <x14:formula1>
             <xm:f>Enums!$B$8:$B$10</xm:f>
           </x14:formula1>
-          <xm:sqref>E4:E6</xm:sqref>
+          <xm:sqref>E6:E8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Enums!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K17</xm:sqref>
+          <xm:sqref>K3:K28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2489,6 +2883,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E81D8C8DDAE8BD44A422697963F06C45" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6816e004dbb89c674e51f5647972552">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2b02348f-b4e3-458c-83fc-9e90db0f8029" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6418ca14ac9ee17b8bbf6df78e0c223" ns2:_="">
     <xsd:import namespace="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
@@ -2646,35 +3055,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCDB6385-31B2-4574-9AA4-BF13B563A4E3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2696,9 +3080,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCDB6385-31B2-4574-9AA4-BF13B563A4E3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
reset to previous commit due to merge error
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE28723-FA94-49FA-A545-4B0FB3072BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8791C450-4F71-402C-AEFD-6027D56F203F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Test Report" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="139">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -87,364 +87,492 @@
   </si>
   <si>
     <t>REQ-04</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-05</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-06</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-07</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>REQ-15</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>High Impact</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Mid Impact</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that the RPI prompts to scan the user's IC, displays "Scan your IC" on the LCD</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that the LCD displays the location and the prompt “Press ‘*’”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>System is powered on and ready</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The LCD displays "Scan your IC" and the camera activates</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that if the barcode corresponds to an account, the user's name and admin number are displayed on the LCD for 1 second</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Valid barcode for an existing account</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The LCD displays the user's name and admin number for 1 second</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test that if the barcode does not correspond to an account, the LCD displays “Please press ‘#’ to try again”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Invalid barcode</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The LCD displays “Please press ‘#’ to try again”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays "Location [1 or 2]" and "Press ‘*’"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-08</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that the LCD displays the main menu options and rotates through the screens</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-09</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “Wrong location. Go to location [1/2]”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-11</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “Maximum books reached (10)”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “Which book to extend loan”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-16</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that the respective names for the lent books are displayed on the LCD, cycling through them if there is more than one book</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD cycles through and displays the names of the lent books</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-17</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “Successfully extended loan”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-18</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that if the selected book has been extended before, the LCD displays “Previously extended”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-19</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The LCD displays “Scan your card to pay fine” and the RFID scanner activates</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that users with unpaid fines are not allowed to borrow any books</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-21</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Scan your card to pay fine” and the RFID scanner activates</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Previously extended”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Successfully extended loan”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD cycles through and displays the names of the lent books</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Which book to extend loan”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Maximum books reached (10)”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Wrong location. Go to location [1/2]”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays and rotates through the menu options</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays “Please press ‘#’ to try again”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays the user's name and admin number for 1 second</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays "Scan your IC" and the camera activates</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD displays "Location [1 or 2]" and "Press ‘*’"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-02</t>
+  </si>
+  <si>
+    <t>Test that the location changes when switch state is changed</t>
+  </si>
+  <si>
+    <t>The LCD displays "Location 1" on line 1 which changes to "Location 2"</t>
+  </si>
+  <si>
+    <t>1. Start the system 
+2. Ensure that the switch is in the left position
+3. Flip the switch to the right position
+4. Check the LCD display</t>
+  </si>
+  <si>
+    <t>System is powered on and ready</t>
+  </si>
+  <si>
+    <t>1. Start the system     
+2. Press '*' on the keypad       
+3. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Place a valid barcode in front of the camera
+2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Place an invalid barcode or no barcode in front of the camera
+2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>Camera is activated and scanning for a barcode</t>
+  </si>
+  <si>
+    <t>1. Check the LCD display</t>
+  </si>
+  <si>
+    <r>
+      <t>The servo motor rotates to 90</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>̊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The DC motor rotates for 5s
+The servo motor rotates to 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>̊</t>
+    </r>
+  </si>
+  <si>
+    <t>Test that when option 3 is pressed, the LCD displays “Which book to extend loan”</t>
+  </si>
+  <si>
+    <t>Test that if more than 10 books have been collected, the system stops dispensing books and the LCD displays “Maximum books reached (10)”</t>
+  </si>
+  <si>
+    <t>Test that if "Collect" is selected and the location is incorrect, the LCD displays “Wrong location. Go to location [1/2]”</t>
+  </si>
+  <si>
+    <t>Test that if "Collect" is selected, the location is checked, and if correct, the book is dispensed</t>
+  </si>
+  <si>
+    <t>1. Press '1' on the keypad  
+2. Verify location is the same location
+3. Check if the motor turn sequence activates, signifying a book being dispensed</t>
+  </si>
+  <si>
+    <t>1. Attempt to collect an 11th book                                              2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Press '3' on the keypad 
+2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Select a book that has not been extended
+2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Select a book that has been extended
+2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Press '4' on the keypad 
+2. Check the LCD display 
+3. Check the RFID scanner activation</t>
+  </si>
+  <si>
+    <t>1. Attempt to borrow a book
+2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Attempt to check fines 
+2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>1. Start the system
+2. Check the LCD display</t>
+  </si>
+  <si>
+    <t>The LCD displays “Previously extended”</t>
+  </si>
+  <si>
+    <t>REQ-26</t>
+  </si>
+  <si>
+    <t>REQ-25</t>
+  </si>
+  <si>
+    <t>Test that if waiting 1min, the program returns to the home page</t>
+  </si>
+  <si>
+    <t>Test that when option 4 is pressed, the LCD displays “Scan your card to pay fine” and activates the RFID scanner</t>
+  </si>
+  <si>
+    <t>Test that when option 5 is pressed, the program returns to the home page</t>
+  </si>
+  <si>
+    <t>User has logged into the system and is at the options page</t>
   </si>
   <si>
     <t>User has logged into the system</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD displays "Location [1 or 2]" and "Press ‘*’"</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-08</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that the LCD displays the main menu options and rotates through the screens</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">User has borrowed a book at a location
+User has logged into the system
+</t>
+  </si>
+  <si>
+    <t>1. Press '1' on the keypad 
+2. Verify location is the other location
+3. Check the LCD</t>
+  </si>
+  <si>
+    <t>User has already collected 10 books
+User has logged into the system</t>
+  </si>
+  <si>
+    <t>User has borrowed books
+User has logged into the system</t>
+  </si>
+  <si>
+    <t>User selects a book that has not been extended before
+User has logged into the system and pressed option 3</t>
+  </si>
+  <si>
+    <t>User selects a book that has been extended before
+User has logged into the system and pressed option 3</t>
+  </si>
+  <si>
+    <t>User has unpaid fines
+User has logged into the system</t>
+  </si>
+  <si>
+    <t>User has no unpaid fines
+User has logged into the system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Press '5' on the keypad 
+2. Check the LCD display </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Wait for 1 minute 
+2. Check the LCD display </t>
+  </si>
+  <si>
+    <t>LCD displays “Time out” and returns to the home page</t>
+  </si>
+  <si>
+    <t>LCD displays “No fine incurred” and returns to the options page</t>
+  </si>
+  <si>
+    <t>LCD displays “Pls pay fine first” and returns to the options page</t>
   </si>
   <si>
     <t>The LCD displays and rotates through the menu options</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-09</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that if "Collect" is selected, the location is checked, and if correct, the book is dispensed</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>User has selected the "Collect" option and is at the correct location</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>The book is dispensed if the user is at the correct location</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-10</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that if "Collect" is selected and the location is incorrect, the LCD displays “Wrong location. Go to location [1/2]”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>User has selected the "Collect" option and is at the wrong location</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD displays “Wrong location. Go to location [1/2]”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-11</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that if more than 10 books have been collected, the system stops dispensing books and the LCD displays “Maximum books reached (10)”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>User has already collected 10 books</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD displays “Maximum books reached (10)”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that when option 3 is pressed, the LCD displays “Which book to extend loan”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>User is on the main menu and selects option 3</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD displays “Which book to extend loan”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-16</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that the respective names for the lent books are displayed on the LCD, cycling through them if there is more than one book</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>User has lent books</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD cycles through and displays the names of the lent books</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-17</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test that if there are no fines, the LCD displays “No fines” before ending the session and returning to the options page</t>
+  </si>
+  <si>
+    <t>LCD returns to the home page</t>
+  </si>
+  <si>
+    <t>REQ-03</t>
+  </si>
+  <si>
+    <t>REQ-01</t>
+  </si>
+  <si>
+    <t>REQ-12</t>
+  </si>
+  <si>
+    <t>REQ-13</t>
+  </si>
+  <si>
+    <t>REQ-14</t>
+  </si>
+  <si>
+    <t>Test that the webpage can be accessed and brings user to sign in page</t>
+  </si>
+  <si>
+    <t>1. Go to IP of the webpage</t>
+  </si>
+  <si>
+    <t>The webpage brings user to the sign in page</t>
+  </si>
+  <si>
+    <t>Internet connected is enabled
+User has not signed in on the webpage</t>
+  </si>
+  <si>
+    <t>Test that the location can be chosen while reserving book</t>
+  </si>
+  <si>
+    <t>1. Go to IP of the webpage
+2. Reserve a book</t>
+  </si>
+  <si>
+    <t>The option of reserving at Location 1 or Location 2 is present</t>
+  </si>
+  <si>
+    <t>The LCD displays borrowed books which can be chosen to return</t>
+  </si>
+  <si>
+    <t>Test that if "Return" is selected, the location is checked, and if correct, the book is dispensed</t>
+  </si>
+  <si>
+    <t>Test that reserved books are automatically removed after 5 days</t>
   </si>
   <si>
     <t>Test that if the selected book has not been extended before, the LCD displays “Successfully extended loan”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>User selects a book that has not been extended before</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD displays “Successfully extended loan”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-18</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that if the selected book has been extended before, the LCD displays “Previously extended”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>User selects a book that has been extended before</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD displays “Previously extended”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-19</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that when option 4 is pressed, the LCD displays “Scan your card to pay fine” and activates the RFID scanner</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>User is on the main menu and selects option 4</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD displays “Scan your card to pay fine” and the RFID scanner activates</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-20</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that users with unpaid fines are not allowed to borrow any books</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>User has unpaid fines</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>The system prevents borrowing and displays an appropriate message if there are unpaid fines</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-21</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test that if there are no fines, the LCD displays “No fines” before ending the session and returning to the main page</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>User has no unpaid fines</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>The LCD displays “No fines” and returns to the main page</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Scan an invalid barcode  2. Check the LCD display</t>
-  </si>
-  <si>
-    <t>1. Attempt to check fines  2. Check the LCD display</t>
-  </si>
-  <si>
-    <t>1. Start the system              2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Scan a valid barcode     2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Navigate to the main menu                                                2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Select the "Collect" option                                                  2. Verify location                                                       3. Check if the book is dispensed</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Select the "Collect" option                                               2. Verify location                               3. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Attempt to collect an 11th book                                              2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Press option 3                             2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Navigate to the loan extension menu                             2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Select a book that has not been extended                            2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Select a book that has been extended                               2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Press option 4                              2. Check the LCD display  3. Check the RFID scanner activation</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Attempt to borrow a book                                        2. Check the LCD display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays “No fines” and returns to the main page</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays “Scan your card to pay fine” and the RFID scanner activates</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays “Previously extended”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays “Successfully extended loan”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD cycles through and displays the names of the lent books</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays “Which book to extend loan”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays “Maximum books reached (10)”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays “Wrong location. Go to location [1/2]”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays and rotates through the menu options</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays “Please press ‘#’ to try again”</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays the user's name and admin number for 1 second</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays "Scan your IC" and the camera activates</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD displays "Location [1 or 2]" and "Press ‘*’"</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">User has reserved a book at a location
+User has logged into the system
+</t>
+  </si>
+  <si>
+    <t>Test that fines are automatically calculated after 18 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User has reserved a book
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User has borrowed a book
+</t>
+  </si>
+  <si>
+    <t>[Software Unit Test]</t>
+  </si>
+  <si>
+    <t>REQ-22</t>
+  </si>
+  <si>
+    <t>REQ-23</t>
+  </si>
+  <si>
+    <t>REQ-24</t>
+  </si>
+  <si>
+    <t>[Non-functional Req]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -452,29 +580,29 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FF333333"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial Unicode MS"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="7">
@@ -542,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -555,18 +683,21 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -599,7 +730,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -661,7 +792,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -811,13 +942,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -883,7 +1014,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -920,7 +1051,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1824,49 +1955,49 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="6">
-        <f>COUNTIF('Test Cases &amp; Results'!B3:B65, "&lt;&gt;")</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+        <f>COUNTIF('Test Cases &amp; Results'!B3:B66, "&lt;&gt;")</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="6">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K67, "Pass")</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K68, "Pass")</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="6">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K67, "Fail")</f>
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K68, "Fail")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="6">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K67, "Not Tested")</f>
-        <v>0</v>
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K68, "Not Tested")</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1875,27 +2006,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:K18"/>
+  <dimension ref="B2:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18:K22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="129" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="28.1796875" customWidth="1"/>
-    <col min="7" max="7" width="21.7265625" customWidth="1"/>
-    <col min="8" max="8" width="25.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.453125" customWidth="1"/>
-    <col min="10" max="10" width="18.54296875" customWidth="1"/>
-    <col min="11" max="11" width="12.54296875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="28.21875" customWidth="1"/>
+    <col min="7" max="7" width="21.77734375" customWidth="1"/>
+    <col min="8" max="8" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1927,486 +2058,753 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="10">
+    <row r="3" spans="2:11" ht="57.6">
+      <c r="B3" s="9">
         <v>1</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>1</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="86.4">
+      <c r="B4" s="9">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="57.6">
+      <c r="B5" s="9">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="43.2">
+      <c r="B6" s="9">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="72">
+      <c r="B7" s="9">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="57.6">
+      <c r="B8" s="9">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="102.6" customHeight="1">
+      <c r="B9" s="9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G9" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="83.4" customHeight="1">
+      <c r="B10" s="9">
+        <v>8</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="G10" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="100.8">
+      <c r="B11" s="9">
+        <v>9</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="86.4">
+      <c r="B12" s="9">
+        <v>10</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="72">
+      <c r="B13" s="9">
+        <v>11</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="86.4">
+      <c r="B14" s="9">
+        <v>12</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="43.2">
+      <c r="B15" s="9">
+        <v>13</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="43.2">
+      <c r="B16" s="9">
+        <v>14</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="43.2">
+      <c r="B17" s="9">
+        <v>15</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="10" t="s">
+      <c r="I17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="72">
+      <c r="B18" s="9">
+        <v>16</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="86.4">
+      <c r="B19" s="9">
+        <v>17</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="86.4">
+      <c r="B20" s="9">
+        <v>18</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="57.6">
+      <c r="B21" s="9">
+        <v>19</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="57.6">
+      <c r="B22" s="9">
+        <v>20</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="57.6">
+      <c r="B23" s="9">
+        <v>21</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="H23" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="K23" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="10">
-        <f>B3+1</f>
-        <v>2</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="10" t="s">
+    <row r="24" spans="2:11">
+      <c r="B24" s="9">
+        <v>22</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11">
+      <c r="B25" s="9">
         <v>23</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="D25" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11">
+      <c r="B26" s="9">
+        <v>24</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="43.2">
+      <c r="B27" s="9">
         <v>25</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="K4" s="8" t="s">
+      <c r="D27" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="K27" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="10">
-        <f t="shared" ref="B5:B17" si="0">B4+1</f>
-        <v>3</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="K5" s="8" t="s">
+    <row r="28" spans="2:11" ht="43.2">
+      <c r="B28" s="9">
+        <v>26</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="K28" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="66" x14ac:dyDescent="0.25">
-      <c r="B6" s="10">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="10">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="66" x14ac:dyDescent="0.25">
-      <c r="B8" s="10">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="66" x14ac:dyDescent="0.25">
-      <c r="B9" s="10">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="10">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="66" x14ac:dyDescent="0.25">
-      <c r="B13" s="10">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" ht="66" x14ac:dyDescent="0.25">
-      <c r="B14" s="10">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" ht="66" x14ac:dyDescent="0.25">
-      <c r="B15" s="10">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" ht="99" x14ac:dyDescent="0.25">
-      <c r="B16" s="10">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" ht="66" x14ac:dyDescent="0.25">
-      <c r="B17" s="10">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="K3:K17">
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="K3:K28">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
@@ -2423,13 +2821,13 @@
           <x14:formula1>
             <xm:f>Enums!$B$8:$B$10</xm:f>
           </x14:formula1>
-          <xm:sqref>E4:E6</xm:sqref>
+          <xm:sqref>E6:E8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Enums!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K17</xm:sqref>
+          <xm:sqref>K3:K28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2445,40 +2843,40 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2">
       <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2">
       <c r="B3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2">
       <c r="B8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2">
       <c r="B9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2">
       <c r="B10" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>